<commit_message>
Edit the date format
</commit_message>
<xml_diff>
--- a/docs/db/printerdata.xlsx
+++ b/docs/db/printerdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_365e\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3947\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2B66C9C-65B6-4353-ACD6-4EF0CCC864C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{253FA8A1-63C5-461E-B5EF-70D03D655699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -47,22 +47,19 @@
     <t>Price</t>
   </si>
   <si>
-    <t>01.07.2019</t>
-  </si>
-  <si>
-    <t>01.08.2019</t>
-  </si>
-  <si>
-    <t>01.09.2019</t>
-  </si>
-  <si>
-    <t>01.10.2019</t>
-  </si>
-  <si>
-    <t>01.11.2019</t>
-  </si>
-  <si>
-    <t>01.01.2019</t>
+    <t>2019-07-01</t>
+  </si>
+  <si>
+    <t>2019-08-01</t>
+  </si>
+  <si>
+    <t>2019-09-01</t>
+  </si>
+  <si>
+    <t>2019-10-01</t>
+  </si>
+  <si>
+    <t>2019-11-01</t>
   </si>
   <si>
     <t>Name</t>
@@ -254,8 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,9 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5843D1EB-E6FB-49EE-97A2-82D7E635D331}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -602,7 +598,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2">
@@ -616,7 +612,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3">
@@ -630,7 +626,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4">
@@ -644,7 +640,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5">
@@ -658,7 +654,7 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6">
@@ -672,7 +668,7 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7">
@@ -686,7 +682,7 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8">
@@ -700,7 +696,7 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9">
@@ -714,7 +710,7 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10">
@@ -728,7 +724,7 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11">
@@ -742,7 +738,7 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12">
@@ -756,7 +752,7 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D13">
@@ -770,7 +766,7 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14">
@@ -784,7 +780,7 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15">
@@ -798,7 +794,7 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16">
@@ -812,7 +808,7 @@
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17">
@@ -826,7 +822,7 @@
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18">
@@ -840,8 +836,8 @@
       <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D19">
         <v>279</v>
@@ -854,7 +850,7 @@
       <c r="B20">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20">
@@ -868,7 +864,7 @@
       <c r="B21">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D21">
@@ -882,7 +878,7 @@
       <c r="B22">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D22">
@@ -896,7 +892,7 @@
       <c r="B23">
         <v>5</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D23">
@@ -910,7 +906,7 @@
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24">
@@ -924,7 +920,7 @@
       <c r="B25">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D25">
@@ -938,7 +934,7 @@
       <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D26">
@@ -952,7 +948,7 @@
       <c r="B27">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D27">
@@ -966,7 +962,7 @@
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D28">
@@ -980,7 +976,7 @@
       <c r="B29">
         <v>6</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D29">
@@ -994,7 +990,7 @@
       <c r="B30">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D30">
@@ -1008,7 +1004,7 @@
       <c r="B31">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D31">
@@ -1022,7 +1018,7 @@
       <c r="B32">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D32">
@@ -1036,7 +1032,7 @@
       <c r="B33">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D33">
@@ -1050,7 +1046,7 @@
       <c r="B34">
         <v>7</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34">
@@ -1064,7 +1060,7 @@
       <c r="B35">
         <v>7</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D35">
@@ -1078,7 +1074,7 @@
       <c r="B36">
         <v>7</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36">
@@ -1092,7 +1088,7 @@
       <c r="B37">
         <v>8</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D37">
@@ -1106,7 +1102,7 @@
       <c r="B38">
         <v>8</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D38">
@@ -1120,7 +1116,7 @@
       <c r="B39">
         <v>8</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D39">
@@ -1134,7 +1130,7 @@
       <c r="B40">
         <v>8</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D40">
@@ -1148,7 +1144,7 @@
       <c r="B41">
         <v>8</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41">
@@ -1162,7 +1158,7 @@
       <c r="B42">
         <v>9</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D42">
@@ -1176,7 +1172,7 @@
       <c r="B43">
         <v>9</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D43">
@@ -1190,7 +1186,7 @@
       <c r="B44">
         <v>9</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D44">
@@ -1204,7 +1200,7 @@
       <c r="B45">
         <v>9</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D45">
@@ -1218,7 +1214,7 @@
       <c r="B46">
         <v>9</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D46">
@@ -1232,7 +1228,7 @@
       <c r="B47">
         <v>10</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D47">
@@ -1246,7 +1242,7 @@
       <c r="B48">
         <v>10</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D48">
@@ -1260,7 +1256,7 @@
       <c r="B49">
         <v>10</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D49">
@@ -1274,7 +1270,7 @@
       <c r="B50">
         <v>10</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D50">
@@ -1288,7 +1284,7 @@
       <c r="B51">
         <v>10</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D51">
@@ -1302,7 +1298,7 @@
       <c r="B52">
         <v>11</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D52">
@@ -1316,7 +1312,7 @@
       <c r="B53">
         <v>11</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D53">
@@ -1330,7 +1326,7 @@
       <c r="B54">
         <v>11</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D54">
@@ -1344,7 +1340,7 @@
       <c r="B55">
         <v>11</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D55">
@@ -1358,7 +1354,7 @@
       <c r="B56">
         <v>11</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D56">
@@ -1372,7 +1368,7 @@
       <c r="B57">
         <v>12</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D57">
@@ -1386,7 +1382,7 @@
       <c r="B58">
         <v>12</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D58">
@@ -1400,7 +1396,7 @@
       <c r="B59">
         <v>12</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D59">
@@ -1414,7 +1410,7 @@
       <c r="B60">
         <v>12</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D60">
@@ -1428,7 +1424,7 @@
       <c r="B61">
         <v>12</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D61">
@@ -1442,7 +1438,7 @@
       <c r="B62">
         <v>13</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D62">
@@ -1456,7 +1452,7 @@
       <c r="B63">
         <v>13</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D63">
@@ -1470,7 +1466,7 @@
       <c r="B64">
         <v>13</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D64">
@@ -1484,7 +1480,7 @@
       <c r="B65">
         <v>13</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65">
@@ -1498,7 +1494,7 @@
       <c r="B66">
         <v>13</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D66">
@@ -1512,7 +1508,7 @@
       <c r="B67">
         <v>14</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D67">
@@ -1526,7 +1522,7 @@
       <c r="B68">
         <v>14</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D68">
@@ -1540,7 +1536,7 @@
       <c r="B69">
         <v>14</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D69">
@@ -1554,7 +1550,7 @@
       <c r="B70">
         <v>14</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D70">
@@ -1568,7 +1564,7 @@
       <c r="B71">
         <v>14</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D71">
@@ -1582,7 +1578,7 @@
       <c r="B72">
         <v>15</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D72">
@@ -1596,7 +1592,7 @@
       <c r="B73">
         <v>15</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D73">
@@ -1610,7 +1606,7 @@
       <c r="B74">
         <v>15</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D74">
@@ -1624,7 +1620,7 @@
       <c r="B75">
         <v>15</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75">
@@ -1638,7 +1634,7 @@
       <c r="B76">
         <v>15</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D76">
@@ -1652,7 +1648,7 @@
       <c r="B77">
         <v>16</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D77">
@@ -1666,7 +1662,7 @@
       <c r="B78">
         <v>16</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D78">
@@ -1680,7 +1676,7 @@
       <c r="B79">
         <v>16</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D79">
@@ -1694,7 +1690,7 @@
       <c r="B80">
         <v>16</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80">
@@ -1708,7 +1704,7 @@
       <c r="B81">
         <v>16</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D81">
@@ -1722,7 +1718,7 @@
       <c r="B82">
         <v>17</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D82">
@@ -1736,7 +1732,7 @@
       <c r="B83">
         <v>17</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D83">
@@ -1750,7 +1746,7 @@
       <c r="B84">
         <v>17</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D84">
@@ -1764,7 +1760,7 @@
       <c r="B85">
         <v>17</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85">
@@ -1778,7 +1774,7 @@
       <c r="B86">
         <v>17</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D86">
@@ -1792,7 +1788,7 @@
       <c r="B87">
         <v>18</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D87">
@@ -1806,7 +1802,7 @@
       <c r="B88">
         <v>18</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D88">
@@ -1820,7 +1816,7 @@
       <c r="B89">
         <v>18</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D89">
@@ -1834,7 +1830,7 @@
       <c r="B90">
         <v>18</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D90">
@@ -1848,7 +1844,7 @@
       <c r="B91">
         <v>18</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D91">
@@ -1862,7 +1858,7 @@
       <c r="B92">
         <v>19</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D92">
@@ -1876,7 +1872,7 @@
       <c r="B93">
         <v>19</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D93">
@@ -1890,7 +1886,7 @@
       <c r="B94">
         <v>19</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D94">
@@ -1904,7 +1900,7 @@
       <c r="B95">
         <v>19</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95">
@@ -1918,7 +1914,7 @@
       <c r="B96">
         <v>19</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D96">
@@ -1932,7 +1928,7 @@
       <c r="B97">
         <v>20</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D97">
@@ -1946,7 +1942,7 @@
       <c r="B98">
         <v>20</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D98">
@@ -1960,7 +1956,7 @@
       <c r="B99">
         <v>20</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D99">
@@ -1974,7 +1970,7 @@
       <c r="B100">
         <v>20</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D100">
@@ -1988,7 +1984,7 @@
       <c r="B101">
         <v>20</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D101">
@@ -2002,7 +1998,7 @@
       <c r="B102">
         <v>21</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D102">
@@ -2016,7 +2012,7 @@
       <c r="B103">
         <v>21</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D103">
@@ -2030,7 +2026,7 @@
       <c r="B104">
         <v>21</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D104">
@@ -2044,7 +2040,7 @@
       <c r="B105">
         <v>21</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D105">
@@ -2058,7 +2054,7 @@
       <c r="B106">
         <v>21</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D106">
@@ -2072,7 +2068,7 @@
       <c r="B107">
         <v>22</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D107">
@@ -2086,7 +2082,7 @@
       <c r="B108">
         <v>22</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D108">
@@ -2100,7 +2096,7 @@
       <c r="B109">
         <v>22</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D109">
@@ -2114,7 +2110,7 @@
       <c r="B110">
         <v>22</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D110">
@@ -2128,7 +2124,7 @@
       <c r="B111">
         <v>22</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D111">
@@ -2142,7 +2138,7 @@
       <c r="B112">
         <v>23</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D112">
@@ -2156,7 +2152,7 @@
       <c r="B113">
         <v>23</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D113">
@@ -2170,7 +2166,7 @@
       <c r="B114">
         <v>23</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D114">
@@ -2184,7 +2180,7 @@
       <c r="B115">
         <v>23</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D115">
@@ -2198,7 +2194,7 @@
       <c r="B116">
         <v>23</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D116">
@@ -2212,7 +2208,7 @@
       <c r="B117">
         <v>24</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D117">
@@ -2226,7 +2222,7 @@
       <c r="B118">
         <v>24</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D118">
@@ -2240,7 +2236,7 @@
       <c r="B119">
         <v>24</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D119">
@@ -2254,7 +2250,7 @@
       <c r="B120">
         <v>24</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D120">
@@ -2268,7 +2264,7 @@
       <c r="B121">
         <v>24</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D121">
@@ -2282,7 +2278,7 @@
       <c r="B122">
         <v>25</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D122">
@@ -2296,7 +2292,7 @@
       <c r="B123">
         <v>25</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D123">
@@ -2310,7 +2306,7 @@
       <c r="B124">
         <v>25</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D124">
@@ -2324,7 +2320,7 @@
       <c r="B125">
         <v>25</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D125">
@@ -2338,7 +2334,7 @@
       <c r="B126">
         <v>25</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D126">
@@ -2352,7 +2348,7 @@
       <c r="B127">
         <v>26</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D127">
@@ -2366,7 +2362,7 @@
       <c r="B128">
         <v>26</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D128">
@@ -2380,7 +2376,7 @@
       <c r="B129">
         <v>26</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D129">
@@ -2394,7 +2390,7 @@
       <c r="B130">
         <v>26</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D130">
@@ -2408,7 +2404,7 @@
       <c r="B131">
         <v>26</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131">
@@ -2422,7 +2418,7 @@
       <c r="B132">
         <v>27</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D132">
@@ -2436,7 +2432,7 @@
       <c r="B133">
         <v>27</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D133">
@@ -2450,7 +2446,7 @@
       <c r="B134">
         <v>27</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D134">
@@ -2464,7 +2460,7 @@
       <c r="B135">
         <v>27</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D135">
@@ -2478,7 +2474,7 @@
       <c r="B136">
         <v>27</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D136">
@@ -2492,7 +2488,7 @@
       <c r="B137">
         <v>28</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D137">
@@ -2506,7 +2502,7 @@
       <c r="B138">
         <v>28</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D138">
@@ -2520,7 +2516,7 @@
       <c r="B139">
         <v>28</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D139">
@@ -2534,7 +2530,7 @@
       <c r="B140">
         <v>28</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D140">
@@ -2548,7 +2544,7 @@
       <c r="B141">
         <v>28</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D141">
@@ -2562,7 +2558,7 @@
       <c r="B142">
         <v>29</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D142">
@@ -2576,7 +2572,7 @@
       <c r="B143">
         <v>29</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D143">
@@ -2590,7 +2586,7 @@
       <c r="B144">
         <v>29</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D144">
@@ -2604,7 +2600,7 @@
       <c r="B145">
         <v>29</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D145">
@@ -2618,7 +2614,7 @@
       <c r="B146">
         <v>29</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D146">
@@ -2632,7 +2628,7 @@
       <c r="B147">
         <v>30</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D147">
@@ -2646,7 +2642,7 @@
       <c r="B148">
         <v>30</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D148">
@@ -2660,7 +2656,7 @@
       <c r="B149">
         <v>30</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D149">
@@ -2674,7 +2670,7 @@
       <c r="B150">
         <v>30</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D150">
@@ -2688,7 +2684,7 @@
       <c r="B151">
         <v>30</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151">
@@ -2704,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2727,37 +2723,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2765,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>468</v>
@@ -2803,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>375</v>
@@ -2841,7 +2837,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>375</v>
@@ -2879,7 +2875,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>375</v>
@@ -2917,7 +2913,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>425</v>
@@ -2955,7 +2951,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>445</v>
@@ -2993,7 +2989,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>438</v>
@@ -3031,7 +3027,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>360</v>
@@ -3069,7 +3065,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>372</v>
@@ -3107,7 +3103,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>454</v>
@@ -3145,7 +3141,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>403</v>
@@ -3183,7 +3179,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>435</v>
@@ -3221,7 +3217,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>464</v>
@@ -3259,7 +3255,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>445</v>
@@ -3297,7 +3293,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>454</v>
@@ -3335,7 +3331,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>400</v>
@@ -3373,7 +3369,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>400</v>
@@ -3411,7 +3407,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>455</v>
@@ -3449,7 +3445,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>390</v>
@@ -3487,7 +3483,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <v>438</v>
@@ -3525,7 +3521,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <v>380</v>
@@ -3563,7 +3559,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>373</v>
@@ -3601,7 +3597,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>479</v>
@@ -3639,7 +3635,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>410</v>
@@ -3677,7 +3673,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26">
         <v>530</v>
@@ -3715,7 +3711,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27">
         <v>463</v>
@@ -3753,7 +3749,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28">
         <v>425</v>
@@ -3791,7 +3787,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>450</v>
@@ -3829,7 +3825,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>435</v>
@@ -3867,7 +3863,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31">
         <v>390</v>
@@ -3918,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3926,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3947,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3955,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3963,7 +3959,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3971,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3979,7 +3975,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4003,10 +3999,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4014,7 +4010,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4025,7 +4021,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4036,7 +4032,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4047,7 +4043,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4062,13 +4058,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C6B4E6-7C04-4825-B835-C122E9ABC65B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4077,10 +4073,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -4091,10 +4087,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -4105,10 +4101,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
       </c>
       <c r="D3">
         <v>98</v>

</xml_diff>